<commit_message>
Tableau d'adressage IP finis + ajout d'un mobile sur le fichier packet tracer
</commit_message>
<xml_diff>
--- a/Table d'adressage IP.xlsx
+++ b/Table d'adressage IP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoann/Desktop/Cours/SAE-3.01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDC3C57B-E054-A542-89FE-0B58222660F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1143E170-33DD-FC4C-9E0E-C2D09578B3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="700" windowWidth="28040" windowHeight="16860" xr2:uid="{92A199EC-D72D-A24C-B8CC-2550C0688723}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="29400" windowHeight="16860" xr2:uid="{92A199EC-D72D-A24C-B8CC-2550C0688723}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
   <si>
     <t>Equipement/Interface</t>
   </si>
@@ -62,9 +62,6 @@
     <t>DNS</t>
   </si>
   <si>
-    <t>Switch</t>
-  </si>
-  <si>
     <t>Port</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>SRV API</t>
   </si>
   <si>
-    <t>Router</t>
-  </si>
-  <si>
     <t>192.168.20.2</t>
   </si>
   <si>
@@ -165,6 +159,21 @@
   </si>
   <si>
     <t>fa0/8</t>
+  </si>
+  <si>
+    <t>Router G0/0/0.10</t>
+  </si>
+  <si>
+    <t>G0/0/0</t>
+  </si>
+  <si>
+    <t>Router G0/0/0.20</t>
+  </si>
+  <si>
+    <t>Router G0/0/0.30</t>
+  </si>
+  <si>
+    <t>192.168.30.1</t>
   </si>
 </sst>
 </file>
@@ -548,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD088E1-35A5-AE45-A127-0B0DFDB3222A}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -589,208 +598,269 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="H4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="E5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="H6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="G7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
La fin la vraie
</commit_message>
<xml_diff>
--- a/Table d'adressage IP.xlsx
+++ b/Table d'adressage IP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoann/Desktop/Cours/SAE-3.01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1143E170-33DD-FC4C-9E0E-C2D09578B3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FB1568-79F2-AD43-89A3-418593A554AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="29400" windowHeight="16860" xr2:uid="{92A199EC-D72D-A24C-B8CC-2550C0688723}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="45">
   <si>
     <t>Equipement/Interface</t>
   </si>
@@ -68,9 +68,6 @@
     <t>PC1</t>
   </si>
   <si>
-    <t>PC2</t>
-  </si>
-  <si>
     <t>SRV API</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>192.168.20.3</t>
   </si>
   <si>
-    <t>VLAn 20</t>
-  </si>
-  <si>
     <t>192.168.20.1</t>
   </si>
   <si>
@@ -174,6 +168,9 @@
   </si>
   <si>
     <t>192.168.30.1</t>
+  </si>
+  <si>
+    <t>SmartPhone</t>
   </si>
 </sst>
 </file>
@@ -560,7 +557,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -606,260 +603,260 @@
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="H4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="E5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="H6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="G7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>